<commit_message>
Assess 2020 with 2019
</commit_message>
<xml_diff>
--- a/inputs - 只有板块.xlsx
+++ b/inputs - 只有板块.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\文档\自然通风组\00 On-The-Go\人力资源部\10 考核\40 考核测算\wagePackage\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12468"/>
+    <workbookView windowWidth="28800" windowHeight="12465"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
   <si>
     <t>var_name</t>
   </si>
@@ -180,46 +175,46 @@
     <t>financial_index_name</t>
   </si>
   <si>
+    <t>JT_compete</t>
+  </si>
+  <si>
+    <t>Compete</t>
+  </si>
+  <si>
+    <t>竞争类板块</t>
+  </si>
+  <si>
+    <t>人均利润</t>
+  </si>
+  <si>
+    <t>人均归母</t>
+  </si>
+  <si>
+    <t>人均营收</t>
+  </si>
+  <si>
+    <t>人均劳动生产总值</t>
+  </si>
+  <si>
+    <t>calculated</t>
+  </si>
+  <si>
+    <t>JT_public</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>公共服务类板块</t>
+  </si>
+  <si>
+    <t>JT_special</t>
+  </si>
+  <si>
     <t>Special</t>
   </si>
   <si>
     <t>Gov</t>
-  </si>
-  <si>
-    <t>人均利润</t>
-  </si>
-  <si>
-    <t>人均营收</t>
-  </si>
-  <si>
-    <t>人均工作量</t>
-  </si>
-  <si>
-    <t>人均劳动生产总值</t>
-  </si>
-  <si>
-    <t>calculated</t>
-  </si>
-  <si>
-    <t>JT_compete</t>
-  </si>
-  <si>
-    <t>竞争类板块</t>
-  </si>
-  <si>
-    <t>Compete</t>
-  </si>
-  <si>
-    <t>JT_public</t>
-  </si>
-  <si>
-    <t>公共服务类板块</t>
-  </si>
-  <si>
-    <t>Public</t>
-  </si>
-  <si>
-    <t>JT_special</t>
   </si>
   <si>
     <t>特殊功能类板块</t>
@@ -228,8 +223,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,14 +247,151 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,12 +406,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor theme="6" tint="0.599993896298105"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -344,9 +668,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -363,6 +929,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -372,19 +939,62 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -642,31 +1252,32 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:BA4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="AV2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozen"/>
+      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AW12" sqref="AW12"/>
+      <selection pane="bottomRight" activeCell="AB22" sqref="AB22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="3" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
-    <col min="5" max="5" width="8.21875" customWidth="1"/>
-    <col min="6" max="19" width="7.21875" customWidth="1"/>
-    <col min="20" max="53" width="8.5546875" customWidth="1"/>
+    <col min="1" max="3" width="10.5583333333333" customWidth="1"/>
+    <col min="4" max="4" width="12.8833333333333" customWidth="1"/>
+    <col min="5" max="5" width="8.21666666666667" customWidth="1"/>
+    <col min="6" max="19" width="7.21666666666667" customWidth="1"/>
+    <col min="20" max="53" width="8.55833333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" s="1" customFormat="1" ht="73.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" s="1" customFormat="1" ht="73.95" customHeight="1" spans="1:53">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -823,351 +1434,366 @@
       <c r="AZ1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BA1" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" ht="15" spans="1:53">
+      <c r="A2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="4">
+        <v>86681</v>
+      </c>
+      <c r="F2" s="4">
+        <v>69023.85</v>
+      </c>
+      <c r="G2" s="4">
+        <v>-17536.17</v>
+      </c>
+      <c r="H2" s="4">
+        <v>3265.54</v>
+      </c>
+      <c r="I2" s="4">
+        <v>-11039.13</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1059234.6</v>
+      </c>
+      <c r="K2" s="4">
+        <v>-96886.33</v>
+      </c>
+      <c r="L2" s="4">
+        <v>964593.58</v>
+      </c>
+      <c r="M2" s="4">
+        <v>-79350.16</v>
+      </c>
+      <c r="N2" s="4">
+        <v>2495.13</v>
+      </c>
+      <c r="O2" s="4">
+        <v>3630.88</v>
+      </c>
+      <c r="P2" s="4">
+        <v>69426.39</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>-29871.96</v>
+      </c>
+      <c r="R2" s="4">
+        <v>17080.19</v>
+      </c>
+      <c r="S2" s="4">
+        <v>-23028.92</v>
+      </c>
+      <c r="T2" s="4">
+        <v>1325445.01</v>
+      </c>
+      <c r="U2" s="4">
+        <v>-87060.54</v>
+      </c>
+      <c r="V2" s="4">
+        <v>1270926.23</v>
+      </c>
+      <c r="W2" s="4">
+        <v>-71500.58</v>
+      </c>
+      <c r="X2" s="4">
+        <v>28596.36</v>
+      </c>
+      <c r="Y2" s="4">
+        <v>2592.58</v>
+      </c>
+      <c r="Z2" s="4">
+        <v>4090.38</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>4131.2838</v>
+      </c>
+      <c r="AB2" s="4">
+        <v>100</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="AH2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AQ2" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="5"/>
+      <c r="AU2" s="5"/>
+      <c r="AV2" s="5"/>
+      <c r="AW2" s="5"/>
+      <c r="AX2" s="5"/>
+      <c r="BA2" s="7"/>
+    </row>
+    <row r="3" spans="1:43">
+      <c r="A3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="7">
-        <v>86681</v>
-      </c>
-      <c r="F2" s="7">
-        <v>69023.850000000006</v>
-      </c>
-      <c r="G2" s="7">
-        <v>-17536.169999999998</v>
-      </c>
-      <c r="H2" s="7">
-        <v>3265.54</v>
-      </c>
-      <c r="I2" s="7">
-        <v>-11039.13</v>
-      </c>
-      <c r="J2" s="7">
-        <v>1059234.6000000001</v>
-      </c>
-      <c r="K2" s="7">
-        <v>-96886.33</v>
-      </c>
-      <c r="L2" s="7">
-        <v>964593.58</v>
-      </c>
-      <c r="M2" s="7">
-        <v>-79350.16</v>
-      </c>
-      <c r="N2" s="7">
-        <v>2495.13</v>
-      </c>
-      <c r="O2" s="7">
-        <v>3630.88</v>
-      </c>
-      <c r="P2" s="7">
-        <v>69426.39</v>
-      </c>
-      <c r="Q2" s="7">
-        <v>-29871.96</v>
-      </c>
-      <c r="R2" s="7">
-        <v>17080.189999999999</v>
-      </c>
-      <c r="S2" s="7">
-        <v>-23028.92</v>
-      </c>
-      <c r="T2" s="7">
-        <v>1325445.01</v>
-      </c>
-      <c r="U2" s="7">
-        <v>-87060.54</v>
-      </c>
-      <c r="V2" s="7">
-        <v>1270926.23</v>
-      </c>
-      <c r="W2" s="7">
-        <v>-71500.58</v>
-      </c>
-      <c r="X2" s="7">
-        <v>28596.36</v>
-      </c>
-      <c r="Y2" s="7">
-        <v>2592.58</v>
-      </c>
-      <c r="Z2" s="7">
-        <v>4090.38</v>
-      </c>
-      <c r="AA2" s="7">
-        <v>4131.2838000000002</v>
-      </c>
-      <c r="AB2" s="7">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="4">
+        <v>40119</v>
+      </c>
+      <c r="F3" s="4">
+        <v>26053</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>11242.95</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4">
+        <v>139991</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4">
+        <v>114395</v>
+      </c>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+      <c r="O3" s="4">
+        <v>455</v>
+      </c>
+      <c r="P3" s="4">
+        <v>8531</v>
+      </c>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4">
+        <v>7199</v>
+      </c>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4">
+        <v>126396</v>
+      </c>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4">
+        <v>118073</v>
+      </c>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4">
+        <v>159</v>
+      </c>
+      <c r="Y3" s="4">
+        <v>49</v>
+      </c>
+      <c r="Z3" s="4">
+        <v>2204</v>
+      </c>
+      <c r="AA3" s="4">
+        <v>2204</v>
+      </c>
+      <c r="AB3" s="4">
         <v>100</v>
       </c>
-      <c r="AC2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AC3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AD3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AE3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AF3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AG3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO3" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AQ3" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52">
+      <c r="A4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="4">
+        <v>61376</v>
+      </c>
+      <c r="F4" s="4">
+        <v>210953.87</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4">
+        <v>191619.85</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4">
+        <v>174949.47</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4">
+        <v>1264057.71</v>
+      </c>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4">
+        <v>336656.46</v>
+      </c>
+      <c r="O4" s="4">
+        <v>971197.1</v>
+      </c>
+      <c r="P4" s="4">
+        <v>250423.05</v>
+      </c>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4">
+        <v>203852.87</v>
+      </c>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4">
+        <v>280140.04</v>
+      </c>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4">
+        <v>1156294.11</v>
+      </c>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4">
+        <v>410463.11</v>
+      </c>
+      <c r="Y4" s="4">
+        <v>701799</v>
+      </c>
+      <c r="Z4" s="4">
+        <v>1981.46</v>
+      </c>
+      <c r="AA4" s="4">
+        <v>1981.46</v>
+      </c>
+      <c r="AB4" s="4">
+        <v>100</v>
+      </c>
+      <c r="AC4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AI2" s="4"/>
-      <c r="AJ2" s="4"/>
-      <c r="AK2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AL2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM2" s="4"/>
-      <c r="AN2" s="4"/>
-      <c r="AO2" s="4">
+      <c r="AG4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO4" s="5">
         <v>0.5</v>
       </c>
-      <c r="AP2" s="4">
+      <c r="AQ4" s="5">
         <v>0.5</v>
       </c>
-      <c r="AQ2" s="4"/>
-      <c r="AR2" s="4"/>
-      <c r="AS2" s="4"/>
-      <c r="AT2" s="4"/>
-      <c r="AU2" s="4"/>
-      <c r="AV2" s="4"/>
-      <c r="AW2" s="4"/>
-      <c r="AX2" s="4"/>
-      <c r="BA2" s="6"/>
-    </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="7">
-        <v>40119</v>
-      </c>
-      <c r="F3" s="7">
-        <v>26053</v>
-      </c>
-      <c r="G3" s="7">
-        <v>0</v>
-      </c>
-      <c r="H3" s="7">
-        <v>11242.95</v>
-      </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7">
-        <v>139991</v>
-      </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7">
-        <v>114395</v>
-      </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7">
-        <v>0</v>
-      </c>
-      <c r="O3" s="7">
-        <v>455</v>
-      </c>
-      <c r="P3" s="7">
-        <v>8531</v>
-      </c>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7">
-        <v>7199</v>
-      </c>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7">
-        <v>126396</v>
-      </c>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7">
-        <v>118073</v>
-      </c>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7">
-        <v>159</v>
-      </c>
-      <c r="Y3" s="7">
-        <v>49</v>
-      </c>
-      <c r="Z3" s="7">
-        <v>2204</v>
-      </c>
-      <c r="AA3" s="7">
-        <v>2204</v>
-      </c>
-      <c r="AB3" s="7">
+      <c r="AY4" s="5">
         <v>100</v>
       </c>
-      <c r="AC3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AL3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO3" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="AP3" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" s="7">
-        <v>61376</v>
-      </c>
-      <c r="F4" s="7">
-        <v>210953.87</v>
-      </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7">
-        <v>191619.85</v>
-      </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7">
-        <v>174949.47</v>
-      </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7">
-        <v>1264057.71</v>
-      </c>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7">
-        <v>336656.46</v>
-      </c>
-      <c r="O4" s="7">
-        <v>971197.1</v>
-      </c>
-      <c r="P4" s="7">
-        <v>250423.05</v>
-      </c>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7">
-        <v>203852.87</v>
-      </c>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7">
-        <v>280140.03999999998</v>
-      </c>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7">
-        <v>1156294.1100000001</v>
-      </c>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7">
-        <v>410463.11</v>
-      </c>
-      <c r="Y4" s="7">
-        <v>701799</v>
-      </c>
-      <c r="Z4" s="7">
-        <v>1981.46</v>
-      </c>
-      <c r="AA4" s="7">
-        <v>1981.46</v>
-      </c>
-      <c r="AB4" s="7">
-        <v>100</v>
-      </c>
-      <c r="AC4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AL4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO4" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="AP4" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="AY4" s="4">
-        <v>100</v>
-      </c>
-      <c r="AZ4" s="4">
+      <c r="AZ4" s="5">
         <v>120</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BA2">
       <formula1>"total_profit,patmi,revenue"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>